<commit_message>
Extract datetimes and times from Excel sheets
</commit_message>
<xml_diff>
--- a/test/files/dates.xlsx
+++ b/test/files/dates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\purch\OneDrive\デスクトップ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8582FD1-79A1-4091-A56E-7E16CC386C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC03B43-8F27-459B-95CC-6C95A214FBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{29AA8263-978F-41D7-9156-0EF63538D802}"/>
   </bookViews>
@@ -33,9 +33,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="181" formatCode="mm/dd/yy;@"/>
-    <numFmt numFmtId="182" formatCode="[$-409]d\-mmm\-yy;@"/>
+  <numFmts count="3">
+    <numFmt numFmtId="176" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="178" formatCode="[$-409]yyyy/m/d\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -76,17 +77,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -403,15 +410,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A084695D-A8D7-40AD-A05D-D6FA63AEFD63}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.375" customWidth="1"/>
+    <col min="1" max="1" width="21.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
@@ -436,6 +443,16 @@
       </c>
       <c r="B3">
         <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="4">
+        <v>44197.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>